<commit_message>
Updated protocol to include empirical calibration
</commit_message>
<xml_diff>
--- a/EvaluatingCaseControl/documents/Tables.xlsx
+++ b/EvaluatingCaseControl/documents/Tables.xlsx
@@ -2460,7 +2460,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D2" sqref="D2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2514,10 +2514,10 @@
         <v>366576</v>
       </c>
       <c r="F2" s="7">
-        <v>1.3421500000000001E-3</v>
+        <v>1.3259999999999999E-3</v>
       </c>
       <c r="G2" s="6">
-        <v>1.2653932130000001</v>
+        <v>1.2670999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2537,10 +2537,10 @@
         <v>27196</v>
       </c>
       <c r="F3" s="7">
-        <v>0.140020591</v>
+        <v>0.14149100000000001</v>
       </c>
       <c r="G3" s="6">
-        <v>1.1128402529999999</v>
+        <v>1.1123449999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>